<commit_message>
Update sidebar styling and append logs
Refactor Streamlit sidebar: remove the old .sidebar-header CSS, replace the sidebar header with inline-styled markup, update divider elements to use <hr> with inline styles, and update the section comment to note the modification. Also include a bumped binary forecast.xlsx (data/regeneration) and append new entries to forecast_log_20260218.log capturing additional model runs and deprecation/warning messages.
</commit_message>
<xml_diff>
--- a/forecast.xlsx
+++ b/forecast.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,13 +463,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="C2" t="n">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D2" t="n">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3">
@@ -479,13 +479,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C3" t="n">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D3" t="n">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="4">
@@ -495,13 +495,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C4" t="n">
-        <v>-140</v>
+        <v>-126</v>
       </c>
       <c r="D4" t="n">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="5">
@@ -511,13 +511,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C5" t="n">
-        <v>-41</v>
+        <v>-54</v>
       </c>
       <c r="D5" t="n">
-        <v>358</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6">
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="C6" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>1018</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="7">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="C7" t="n">
-        <v>-43</v>
+        <v>-47</v>
       </c>
       <c r="D7" t="n">
-        <v>957</v>
+        <v>941</v>
       </c>
     </row>
     <row r="8">
@@ -559,13 +559,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>861</v>
+        <v>840</v>
       </c>
     </row>
     <row r="9">
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="C9" t="n">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="D9" t="n">
-        <v>547</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10">
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C10" t="n">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D10" t="n">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="11">
@@ -607,13 +607,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C11" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D11" t="n">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12">
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C12" t="n">
-        <v>-36</v>
+        <v>-3</v>
       </c>
       <c r="D12" t="n">
-        <v>241</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13">
@@ -639,13 +639,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="C13" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>1004</v>
+        <v>985</v>
       </c>
     </row>
     <row r="14">
@@ -655,13 +655,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="C14" t="n">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D14" t="n">
-        <v>766</v>
+        <v>755</v>
       </c>
     </row>
     <row r="15">
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="C15" t="n">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="D15" t="n">
-        <v>701</v>
+        <v>686</v>
       </c>
     </row>
     <row r="16">
@@ -687,13 +687,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="C16" t="n">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D16" t="n">
-        <v>565</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17">
@@ -703,10 +703,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C17" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D17" t="n">
         <v>625</v>
@@ -719,13 +719,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C18" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D18" t="n">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19">
@@ -735,13 +735,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C19" t="n">
-        <v>-7</v>
+        <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>225</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20">
@@ -751,13 +751,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>517</v>
+        <v>501</v>
       </c>
       <c r="C20" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D20" t="n">
-        <v>989</v>
+        <v>970</v>
       </c>
     </row>
     <row r="21">
@@ -767,13 +767,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>519</v>
+        <v>503</v>
       </c>
       <c r="C21" t="n">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="D21" t="n">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="22">
@@ -783,13 +783,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="C22" t="n">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="D22" t="n">
-        <v>694</v>
+        <v>684</v>
       </c>
     </row>
     <row r="23">
@@ -799,13 +799,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="C23" t="n">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D23" t="n">
-        <v>612</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24">
@@ -815,10 +815,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C24" t="n">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D24" t="n">
         <v>673</v>
@@ -831,13 +831,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C25" t="n">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D25" t="n">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26">
@@ -847,13 +847,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="C26" t="n">
-        <v>-8</v>
+        <v>39</v>
       </c>
       <c r="D26" t="n">
-        <v>254</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27">
@@ -863,13 +863,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>518</v>
+        <v>499</v>
       </c>
       <c r="C27" t="n">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D27" t="n">
-        <v>996</v>
+        <v>979</v>
       </c>
     </row>
     <row r="28">
@@ -879,13 +879,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="C28" t="n">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="D28" t="n">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="29">
@@ -895,13 +895,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="C29" t="n">
-        <v>257</v>
+        <v>225</v>
       </c>
       <c r="D29" t="n">
-        <v>707</v>
+        <v>701</v>
       </c>
     </row>
     <row r="30">
@@ -911,13 +911,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="C30" t="n">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="D30" t="n">
-        <v>630</v>
+        <v>608</v>
       </c>
     </row>
     <row r="31">
@@ -927,13 +927,973 @@
         </is>
       </c>
       <c r="B31" t="n">
+        <v>437</v>
+      </c>
+      <c r="C31" t="n">
+        <v>207</v>
+      </c>
+      <c r="D31" t="n">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-02-28</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>183</v>
+      </c>
+      <c r="C32" t="n">
+        <v>50</v>
+      </c>
+      <c r="D32" t="n">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-03-01</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>97</v>
+      </c>
+      <c r="C33" t="n">
+        <v>44</v>
+      </c>
+      <c r="D33" t="n">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-03-02</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>494</v>
+      </c>
+      <c r="C34" t="n">
+        <v>9</v>
+      </c>
+      <c r="D34" t="n">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-03-03</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>497</v>
+      </c>
+      <c r="C35" t="n">
+        <v>236</v>
+      </c>
+      <c r="D35" t="n">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-03-04</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>462</v>
+      </c>
+      <c r="C36" t="n">
+        <v>232</v>
+      </c>
+      <c r="D36" t="n">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-03-05</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>411</v>
+      </c>
+      <c r="C37" t="n">
+        <v>233</v>
+      </c>
+      <c r="D37" t="n">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-03-06</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>434</v>
+      </c>
+      <c r="C38" t="n">
+        <v>212</v>
+      </c>
+      <c r="D38" t="n">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-03-07</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>179</v>
+      </c>
+      <c r="C39" t="n">
+        <v>40</v>
+      </c>
+      <c r="D39" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-03-08</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>92</v>
+      </c>
+      <c r="C40" t="n">
+        <v>30</v>
+      </c>
+      <c r="D40" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-03-09</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>488</v>
+      </c>
+      <c r="C41" t="n">
+        <v>5</v>
+      </c>
+      <c r="D41" t="n">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-03-10</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>495</v>
+      </c>
+      <c r="C42" t="n">
+        <v>243</v>
+      </c>
+      <c r="D42" t="n">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-03-11</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>459</v>
+      </c>
+      <c r="C43" t="n">
+        <v>236</v>
+      </c>
+      <c r="D43" t="n">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-03-12</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>409</v>
+      </c>
+      <c r="C44" t="n">
+        <v>239</v>
+      </c>
+      <c r="D44" t="n">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-03-13</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>431</v>
+      </c>
+      <c r="C45" t="n">
+        <v>206</v>
+      </c>
+      <c r="D45" t="n">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-03-14</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>176</v>
+      </c>
+      <c r="C46" t="n">
+        <v>33</v>
+      </c>
+      <c r="D46" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-03-15</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>93</v>
+      </c>
+      <c r="C47" t="n">
+        <v>30</v>
+      </c>
+      <c r="D47" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-03-16</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>487</v>
+      </c>
+      <c r="C48" t="n">
+        <v>9</v>
+      </c>
+      <c r="D48" t="n">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-03-17</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>496</v>
+      </c>
+      <c r="C49" t="n">
+        <v>243</v>
+      </c>
+      <c r="D49" t="n">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-03-18</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>460</v>
+      </c>
+      <c r="C50" t="n">
+        <v>231</v>
+      </c>
+      <c r="D50" t="n">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-03-19</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>411</v>
+      </c>
+      <c r="C51" t="n">
+        <v>230</v>
+      </c>
+      <c r="D51" t="n">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-03-20</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>435</v>
+      </c>
+      <c r="C52" t="n">
+        <v>207</v>
+      </c>
+      <c r="D52" t="n">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-03-21</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>183</v>
+      </c>
+      <c r="C53" t="n">
+        <v>27</v>
+      </c>
+      <c r="D53" t="n">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-03-22</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>100</v>
+      </c>
+      <c r="C54" t="n">
+        <v>51</v>
+      </c>
+      <c r="D54" t="n">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-03-23</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>490</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D55" t="n">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-03-24</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>501</v>
+      </c>
+      <c r="C56" t="n">
+        <v>234</v>
+      </c>
+      <c r="D56" t="n">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-03-25</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>466</v>
+      </c>
+      <c r="C57" t="n">
+        <v>221</v>
+      </c>
+      <c r="D57" t="n">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-03-26</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>417</v>
+      </c>
+      <c r="C58" t="n">
+        <v>216</v>
+      </c>
+      <c r="D58" t="n">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-03-27</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
         <v>436</v>
       </c>
-      <c r="C31" t="n">
-        <v>204</v>
-      </c>
-      <c r="D31" t="n">
-        <v>667</v>
+      <c r="C59" t="n">
+        <v>184</v>
+      </c>
+      <c r="D59" t="n">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-03-28</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>186</v>
+      </c>
+      <c r="C60" t="n">
+        <v>39</v>
+      </c>
+      <c r="D60" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-03-29</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>107</v>
+      </c>
+      <c r="C61" t="n">
+        <v>78</v>
+      </c>
+      <c r="D61" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-03-30</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>492</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-11</v>
+      </c>
+      <c r="D62" t="n">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-03-31</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>506</v>
+      </c>
+      <c r="C63" t="n">
+        <v>224</v>
+      </c>
+      <c r="D63" t="n">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-04-01</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>470</v>
+      </c>
+      <c r="C64" t="n">
+        <v>210</v>
+      </c>
+      <c r="D64" t="n">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-04-02</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>426</v>
+      </c>
+      <c r="C65" t="n">
+        <v>220</v>
+      </c>
+      <c r="D65" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-04-03</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>439</v>
+      </c>
+      <c r="C66" t="n">
+        <v>173</v>
+      </c>
+      <c r="D66" t="n">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-04-04</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>191</v>
+      </c>
+      <c r="C67" t="n">
+        <v>30</v>
+      </c>
+      <c r="D67" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-04-05</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>115</v>
+      </c>
+      <c r="C68" t="n">
+        <v>83</v>
+      </c>
+      <c r="D68" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-04-06</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>493</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-7</v>
+      </c>
+      <c r="D69" t="n">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-04-07</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>510</v>
+      </c>
+      <c r="C70" t="n">
+        <v>231</v>
+      </c>
+      <c r="D70" t="n">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-04-08</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>476</v>
+      </c>
+      <c r="C71" t="n">
+        <v>225</v>
+      </c>
+      <c r="D71" t="n">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-04-09</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>426</v>
+      </c>
+      <c r="C72" t="n">
+        <v>219</v>
+      </c>
+      <c r="D72" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-04-10</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>437</v>
+      </c>
+      <c r="C73" t="n">
+        <v>160</v>
+      </c>
+      <c r="D73" t="n">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-04-11</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>193</v>
+      </c>
+      <c r="C74" t="n">
+        <v>12</v>
+      </c>
+      <c r="D74" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-04-12</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>122</v>
+      </c>
+      <c r="C75" t="n">
+        <v>58</v>
+      </c>
+      <c r="D75" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-04-13</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>491</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-6</v>
+      </c>
+      <c r="D76" t="n">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2026-04-14</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>512</v>
+      </c>
+      <c r="C77" t="n">
+        <v>239</v>
+      </c>
+      <c r="D77" t="n">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2026-04-15</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>480</v>
+      </c>
+      <c r="C78" t="n">
+        <v>237</v>
+      </c>
+      <c r="D78" t="n">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2026-04-16</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>429</v>
+      </c>
+      <c r="C79" t="n">
+        <v>226</v>
+      </c>
+      <c r="D79" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2026-04-17</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>434</v>
+      </c>
+      <c r="C80" t="n">
+        <v>136</v>
+      </c>
+      <c r="D80" t="n">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2026-04-18</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>197</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-11</v>
+      </c>
+      <c r="D81" t="n">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2026-04-19</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>134</v>
+      </c>
+      <c r="C82" t="n">
+        <v>22</v>
+      </c>
+      <c r="D82" t="n">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2026-04-20</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>491</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-7</v>
+      </c>
+      <c r="D83" t="n">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2026-04-21</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>520</v>
+      </c>
+      <c r="C84" t="n">
+        <v>244</v>
+      </c>
+      <c r="D84" t="n">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2026-04-22</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>485</v>
+      </c>
+      <c r="C85" t="n">
+        <v>233</v>
+      </c>
+      <c r="D85" t="n">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2026-04-23</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>432</v>
+      </c>
+      <c r="C86" t="n">
+        <v>212</v>
+      </c>
+      <c r="D86" t="n">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2026-04-24</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>429</v>
+      </c>
+      <c r="C87" t="n">
+        <v>80</v>
+      </c>
+      <c r="D87" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2026-04-25</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>203</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-13</v>
+      </c>
+      <c r="D88" t="n">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2026-04-26</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>156</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-17</v>
+      </c>
+      <c r="D89" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2026-04-27</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>498</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-12</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2026-04-28</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>531</v>
+      </c>
+      <c r="C91" t="n">
+        <v>233</v>
+      </c>
+      <c r="D91" t="n">
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -1026,10 +1986,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>65.42857142857143</v>
+        <v>78.42857142857143</v>
       </c>
       <c r="C6" t="n">
-        <v>74.33803102815448</v>
+        <v>91.74576673768503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>